<commit_message>
Update Code Group, Add Name
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C44475
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/CodeGroupTemplate.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/CodeGroupTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samer.haidar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\TOneV2\Code\TOneV2\TOne.WhS.BusinessEntity.Web\WhS_BusinessEntity\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Code Group</t>
   </si>
@@ -36,12 +36,21 @@
   </si>
   <si>
     <t>Syria</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Lebanon Gov</t>
+  </si>
+  <si>
+    <t>Syria 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -359,41 +368,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>961</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>962</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing sirya from code group template
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C46672
</commit_message>
<xml_diff>
--- a/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/CodeGroupTemplate.xlsx
+++ b/TOneV2/Code/TOneV2/TOne.WhS.BusinessEntity.Web/WhS_BusinessEntity/Templates/CodeGroupTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Code Group</t>
   </si>
@@ -35,22 +35,16 @@
     <t>Lebanon</t>
   </si>
   <si>
-    <t>Syria</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Lebanon Gov</t>
   </si>
-  <si>
-    <t>Syria 1</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,11 +362,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -390,7 +384,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -401,18 +395,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>962</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>